<commit_message>
chore: updated analysis services and powerbi
</commit_message>
<xml_diff>
--- a/Integration Services/Trabalho-SNS-Dadores-Sangue/dadoresdesangue.xlsx
+++ b/Integration Services/Trabalho-SNS-Dadores-Sangue/dadoresdesangue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\university\Integration Services\Trabalho-SNS-Dadores-Sangue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1DFED2-2841-49B3-9909-F51B4314073E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0494E222-252B-4C77-9244-247B988EFA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{2903C878-7FFF-4CA2-B62B-0D210148B0EF}"/>
   </bookViews>
@@ -248,7 +248,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-816]mmmmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-816]mmmmm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -281,7 +281,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,7 +699,7 @@
         <v>407</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:J66" si="0">MONTH(DATEVALUE(B3&amp;"1"))</f>
+        <f t="shared" ref="I3:I66" si="0">MONTH(DATEVALUE(B3&amp;"1"))</f>
         <v>1</v>
       </c>
     </row>
@@ -2619,7 +2619,7 @@
         <v>173</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:J130" si="1">MONTH(DATEVALUE(B67&amp;"1"))</f>
+        <f t="shared" ref="I67:I130" si="1">MONTH(DATEVALUE(B67&amp;"1"))</f>
         <v>5</v>
       </c>
     </row>
@@ -4539,7 +4539,7 @@
         <v>435</v>
       </c>
       <c r="I131">
-        <f t="shared" ref="I131:J194" si="2">MONTH(DATEVALUE(B131&amp;"1"))</f>
+        <f t="shared" ref="I131:I194" si="2">MONTH(DATEVALUE(B131&amp;"1"))</f>
         <v>11</v>
       </c>
     </row>
@@ -6459,7 +6459,7 @@
         <v>366</v>
       </c>
       <c r="I195">
-        <f t="shared" ref="I195:J258" si="3">MONTH(DATEVALUE(B195&amp;"1"))</f>
+        <f t="shared" ref="I195:I258" si="3">MONTH(DATEVALUE(B195&amp;"1"))</f>
         <v>9</v>
       </c>
     </row>
@@ -8379,7 +8379,7 @@
         <v>578</v>
       </c>
       <c r="I259">
-        <f t="shared" ref="I259:J322" si="4">MONTH(DATEVALUE(B259&amp;"1"))</f>
+        <f t="shared" ref="I259:I322" si="4">MONTH(DATEVALUE(B259&amp;"1"))</f>
         <v>3</v>
       </c>
     </row>
@@ -10299,7 +10299,7 @@
         <v>375</v>
       </c>
       <c r="I323">
-        <f t="shared" ref="I323:J386" si="5">MONTH(DATEVALUE(B323&amp;"1"))</f>
+        <f t="shared" ref="I323:I386" si="5">MONTH(DATEVALUE(B323&amp;"1"))</f>
         <v>7</v>
       </c>
     </row>
@@ -12219,7 +12219,7 @@
         <v>476</v>
       </c>
       <c r="I387">
-        <f t="shared" ref="I387:J450" si="6">MONTH(DATEVALUE(B387&amp;"1"))</f>
+        <f t="shared" ref="I387:I450" si="6">MONTH(DATEVALUE(B387&amp;"1"))</f>
         <v>2</v>
       </c>
     </row>
@@ -14139,7 +14139,7 @@
         <v>128</v>
       </c>
       <c r="I451">
-        <f t="shared" ref="I451:J514" si="7">MONTH(DATEVALUE(B451&amp;"1"))</f>
+        <f t="shared" ref="I451:I514" si="7">MONTH(DATEVALUE(B451&amp;"1"))</f>
         <v>7</v>
       </c>
     </row>
@@ -16059,7 +16059,7 @@
         <v>531</v>
       </c>
       <c r="I515">
-        <f t="shared" ref="I515:J578" si="8">MONTH(DATEVALUE(B515&amp;"1"))</f>
+        <f t="shared" ref="I515:I578" si="8">MONTH(DATEVALUE(B515&amp;"1"))</f>
         <v>5</v>
       </c>
     </row>
@@ -17979,7 +17979,7 @@
         <v>365</v>
       </c>
       <c r="I579">
-        <f t="shared" ref="I579:J642" si="9">MONTH(DATEVALUE(B579&amp;"1"))</f>
+        <f t="shared" ref="I579:I642" si="9">MONTH(DATEVALUE(B579&amp;"1"))</f>
         <v>9</v>
       </c>
     </row>
@@ -19899,7 +19899,7 @@
         <v>894</v>
       </c>
       <c r="I643">
-        <f t="shared" ref="I643:J706" si="10">MONTH(DATEVALUE(B643&amp;"1"))</f>
+        <f t="shared" ref="I643:I706" si="10">MONTH(DATEVALUE(B643&amp;"1"))</f>
         <v>1</v>
       </c>
     </row>
@@ -21819,7 +21819,7 @@
         <v>51</v>
       </c>
       <c r="I707">
-        <f t="shared" ref="I707:J770" si="11">MONTH(DATEVALUE(B707&amp;"1"))</f>
+        <f t="shared" ref="I707:I770" si="11">MONTH(DATEVALUE(B707&amp;"1"))</f>
         <v>8</v>
       </c>
     </row>
@@ -23739,7 +23739,7 @@
         <v>1091</v>
       </c>
       <c r="I771">
-        <f t="shared" ref="I771:J834" si="12">MONTH(DATEVALUE(B771&amp;"1"))</f>
+        <f t="shared" ref="I771:I834" si="12">MONTH(DATEVALUE(B771&amp;"1"))</f>
         <v>2</v>
       </c>
     </row>
@@ -25659,7 +25659,7 @@
         <v>377</v>
       </c>
       <c r="I835">
-        <f t="shared" ref="I835:J898" si="13">MONTH(DATEVALUE(B835&amp;"1"))</f>
+        <f t="shared" ref="I835:I837" si="13">MONTH(DATEVALUE(B835&amp;"1"))</f>
         <v>6</v>
       </c>
     </row>
@@ -25734,10 +25734,17 @@
   <dimension ref="A1:I837"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>